<commit_message>
Minor test data corrections
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_CA_CHOICE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Desktop\SUITE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -309,9 +309,6 @@
     <t>TOYOTA</t>
   </si>
   <si>
-    <t>BBBKN3DD&amp;E</t>
-  </si>
-  <si>
     <t>MAKEPAS2713ENDOR</t>
   </si>
   <si>
@@ -328,6 +325,9 @@
   </si>
   <si>
     <t>AAAVB3CC&amp;W</t>
+  </si>
+  <si>
+    <t>GGGVB2CC&amp;W</t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,7 @@
   <dimension ref="A1:AL9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +841,7 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>73</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>73</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>73</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>73</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>73</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>73</v>
@@ -1546,16 +1546,16 @@
         <v>2018</v>
       </c>
       <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
         <v>76</v>
       </c>
-      <c r="E8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>77</v>
-      </c>
-      <c r="G8" t="s">
-        <v>78</v>
       </c>
       <c r="H8" s="3">
         <v>88888</v>
@@ -1564,13 +1564,13 @@
         <v>29</v>
       </c>
       <c r="J8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>64</v>
       </c>
       <c r="L8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>29</v>

</xml_diff>